<commit_message>
update dash sub borrow
</commit_message>
<xml_diff>
--- a/Aluguel/stream-dash/devolucao.xlsx
+++ b/Aluguel/stream-dash/devolucao.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="103">
   <si>
     <t>Data</t>
   </si>
@@ -88,6 +88,9 @@
     <t>CPFE3</t>
   </si>
   <si>
+    <t>CYRE3</t>
+  </si>
+  <si>
     <t>EMBR3</t>
   </si>
   <si>
@@ -112,6 +115,9 @@
     <t>IGTI11</t>
   </si>
   <si>
+    <t>LWSA3</t>
+  </si>
+  <si>
     <t>MOVI3</t>
   </si>
   <si>
@@ -166,6 +172,39 @@
     <t>2022031100335900250001-1</t>
   </si>
   <si>
+    <t>2022040100340127810001-1</t>
+  </si>
+  <si>
+    <t>2022040100340127820001-1</t>
+  </si>
+  <si>
+    <t>2022040100340127830001-1</t>
+  </si>
+  <si>
+    <t>2022040100340127850001-1</t>
+  </si>
+  <si>
+    <t>2022022400333117240001-1</t>
+  </si>
+  <si>
+    <t>2022030300333891860001-1</t>
+  </si>
+  <si>
+    <t>2022031000321886990001-2</t>
+  </si>
+  <si>
+    <t>2022031000321887010001-2</t>
+  </si>
+  <si>
+    <t>2022030400334400740001-1</t>
+  </si>
+  <si>
+    <t>2022030900335288940001-1</t>
+  </si>
+  <si>
+    <t>2022030900335342430001-1</t>
+  </si>
+  <si>
     <t>2022030900335295750001-1</t>
   </si>
   <si>
@@ -211,6 +250,12 @@
     <t>2022022400332989380001-1</t>
   </si>
   <si>
+    <t>2022010500323158650001-1</t>
+  </si>
+  <si>
+    <t>2022040100340228730001-1</t>
+  </si>
+  <si>
     <t>2022022300332767120001-1</t>
   </si>
   <si>
@@ -224,6 +269,24 @@
   </si>
   <si>
     <t>2022040100340230510001-1</t>
+  </si>
+  <si>
+    <t>2022040100340230610001-1</t>
+  </si>
+  <si>
+    <t>2022040100340230710001-1</t>
+  </si>
+  <si>
+    <t>2022040100340230790001-1</t>
+  </si>
+  <si>
+    <t>2022040100340230930001-1</t>
+  </si>
+  <si>
+    <t>2022040100340231040001-1</t>
+  </si>
+  <si>
+    <t>2022040100340231060001-1</t>
   </si>
   <si>
     <t>2022040100340229380001-1</t>
@@ -621,7 +684,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M45"/>
+  <dimension ref="A1:M64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -697,7 +760,7 @@
         <v>19</v>
       </c>
       <c r="K2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="L2">
         <v>1400</v>
@@ -738,7 +801,7 @@
         <v>19</v>
       </c>
       <c r="K3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="L3">
         <v>479</v>
@@ -779,7 +842,7 @@
         <v>19</v>
       </c>
       <c r="K4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="L4">
         <v>1900</v>
@@ -820,7 +883,7 @@
         <v>20</v>
       </c>
       <c r="K5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="L5">
         <v>300</v>
@@ -861,7 +924,7 @@
         <v>20</v>
       </c>
       <c r="K6" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="L6">
         <v>2300</v>
@@ -902,7 +965,7 @@
         <v>20</v>
       </c>
       <c r="K7" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="L7">
         <v>6400</v>
@@ -943,7 +1006,7 @@
         <v>20</v>
       </c>
       <c r="K8" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="L8">
         <v>1301</v>
@@ -984,7 +1047,7 @@
         <v>21</v>
       </c>
       <c r="K9" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="L9">
         <v>334</v>
@@ -1025,7 +1088,7 @@
         <v>22</v>
       </c>
       <c r="K10" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="L10">
         <v>400</v>
@@ -1066,7 +1129,7 @@
         <v>22</v>
       </c>
       <c r="K11" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="L11">
         <v>4800</v>
@@ -1107,7 +1170,7 @@
         <v>22</v>
       </c>
       <c r="K12" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="L12">
         <v>1800</v>
@@ -1148,7 +1211,7 @@
         <v>23</v>
       </c>
       <c r="K13" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="L13">
         <v>123</v>
@@ -1162,7 +1225,7 @@
         <v>19</v>
       </c>
       <c r="B14" s="2">
-        <v>44629</v>
+        <v>44652</v>
       </c>
       <c r="C14" t="s">
         <v>12</v>
@@ -1174,13 +1237,13 @@
         <v>17</v>
       </c>
       <c r="F14" s="2">
-        <v>44670</v>
+        <v>44694</v>
       </c>
       <c r="G14">
-        <v>1.35</v>
+        <v>16.75</v>
       </c>
       <c r="H14">
-        <v>15.65</v>
+        <v>17.59</v>
       </c>
       <c r="I14" t="s">
         <v>18</v>
@@ -1189,13 +1252,13 @@
         <v>24</v>
       </c>
       <c r="K14" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="L14">
-        <v>1600</v>
+        <v>1028</v>
       </c>
       <c r="M14">
-        <v>1600</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="15" spans="1:13">
@@ -1203,7 +1266,7 @@
         <v>20</v>
       </c>
       <c r="B15" s="2">
-        <v>44631</v>
+        <v>44652</v>
       </c>
       <c r="C15" t="s">
         <v>12</v>
@@ -1215,13 +1278,13 @@
         <v>17</v>
       </c>
       <c r="F15" s="2">
-        <v>44673</v>
+        <v>44694</v>
       </c>
       <c r="G15">
-        <v>1.29</v>
+        <v>16.75</v>
       </c>
       <c r="H15">
-        <v>14.36</v>
+        <v>17.59</v>
       </c>
       <c r="I15" t="s">
         <v>18</v>
@@ -1230,13 +1293,13 @@
         <v>24</v>
       </c>
       <c r="K15" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="L15">
-        <v>1600</v>
+        <v>127</v>
       </c>
       <c r="M15">
-        <v>1600</v>
+        <v>127</v>
       </c>
     </row>
     <row r="16" spans="1:13">
@@ -1244,7 +1307,7 @@
         <v>21</v>
       </c>
       <c r="B16" s="2">
-        <v>44651</v>
+        <v>44652</v>
       </c>
       <c r="C16" t="s">
         <v>12</v>
@@ -1256,13 +1319,13 @@
         <v>17</v>
       </c>
       <c r="F16" s="2">
-        <v>44693</v>
+        <v>44694</v>
       </c>
       <c r="G16">
-        <v>0.8699999999999999</v>
+        <v>16.75</v>
       </c>
       <c r="H16">
-        <v>15.41</v>
+        <v>17.59</v>
       </c>
       <c r="I16" t="s">
         <v>18</v>
@@ -1271,13 +1334,13 @@
         <v>24</v>
       </c>
       <c r="K16" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="L16">
-        <v>544</v>
+        <v>698</v>
       </c>
       <c r="M16">
-        <v>544</v>
+        <v>698</v>
       </c>
     </row>
     <row r="17" spans="1:13">
@@ -1285,7 +1348,7 @@
         <v>22</v>
       </c>
       <c r="B17" s="2">
-        <v>44651</v>
+        <v>44652</v>
       </c>
       <c r="C17" t="s">
         <v>12</v>
@@ -1297,13 +1360,13 @@
         <v>17</v>
       </c>
       <c r="F17" s="2">
-        <v>44693</v>
+        <v>44694</v>
       </c>
       <c r="G17">
-        <v>0.8699999999999999</v>
+        <v>16.75</v>
       </c>
       <c r="H17">
-        <v>15.41</v>
+        <v>17.59</v>
       </c>
       <c r="I17" t="s">
         <v>18</v>
@@ -1312,59 +1375,59 @@
         <v>24</v>
       </c>
       <c r="K17" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="L17">
-        <v>3300</v>
+        <v>180</v>
       </c>
       <c r="M17">
-        <v>2900</v>
+        <v>180</v>
       </c>
     </row>
     <row r="18" spans="1:13">
       <c r="A18" s="1">
+        <v>23</v>
+      </c>
+      <c r="B18" s="2">
+        <v>44616</v>
+      </c>
+      <c r="C18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" t="s">
+        <v>17</v>
+      </c>
+      <c r="F18" s="2">
+        <v>44658</v>
+      </c>
+      <c r="G18">
+        <v>1.6</v>
+      </c>
+      <c r="H18">
+        <v>15.57</v>
+      </c>
+      <c r="I18" t="s">
+        <v>18</v>
+      </c>
+      <c r="J18" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="2">
-        <v>44629</v>
-      </c>
-      <c r="C18" t="s">
-        <v>12</v>
-      </c>
-      <c r="D18" t="s">
-        <v>14</v>
-      </c>
-      <c r="E18" t="s">
-        <v>17</v>
-      </c>
-      <c r="F18" s="2">
-        <v>44670</v>
-      </c>
-      <c r="G18">
-        <v>2.9</v>
-      </c>
-      <c r="H18">
-        <v>20.73</v>
-      </c>
-      <c r="I18" t="s">
-        <v>18</v>
-      </c>
-      <c r="J18" t="s">
-        <v>25</v>
-      </c>
       <c r="K18" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="L18">
-        <v>1300</v>
+        <v>1200</v>
       </c>
       <c r="M18">
-        <v>1300</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="19" spans="1:13">
       <c r="A19" s="1">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B19" s="2">
         <v>44623</v>
@@ -1382,115 +1445,115 @@
         <v>44663</v>
       </c>
       <c r="G19">
-        <v>7.199999999999999</v>
+        <v>1.6</v>
       </c>
       <c r="H19">
-        <v>17.65</v>
+        <v>14.95</v>
       </c>
       <c r="I19" t="s">
         <v>18</v>
       </c>
       <c r="J19" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="K19" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="L19">
-        <v>350</v>
+        <v>100</v>
       </c>
       <c r="M19">
-        <v>350</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:13">
       <c r="A20" s="1">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B20" s="2">
-        <v>44631</v>
+        <v>44630</v>
       </c>
       <c r="C20" t="s">
         <v>12</v>
       </c>
       <c r="D20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E20" t="s">
         <v>17</v>
       </c>
       <c r="F20" s="2">
-        <v>44673</v>
+        <v>44671</v>
       </c>
       <c r="G20">
-        <v>6.84</v>
+        <v>1.65</v>
       </c>
       <c r="H20">
-        <v>16.99</v>
+        <v>14.42</v>
       </c>
       <c r="I20" t="s">
         <v>18</v>
       </c>
       <c r="J20" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="K20" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="L20">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="M20">
-        <v>100</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:13">
       <c r="A21" s="1">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B21" s="2">
-        <v>44629</v>
+        <v>44630</v>
       </c>
       <c r="C21" t="s">
         <v>12</v>
       </c>
       <c r="D21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E21" t="s">
         <v>17</v>
       </c>
       <c r="F21" s="2">
-        <v>44670</v>
+        <v>44671</v>
       </c>
       <c r="G21">
-        <v>6.84</v>
+        <v>1.65</v>
       </c>
       <c r="H21">
-        <v>16.33</v>
+        <v>14.42</v>
       </c>
       <c r="I21" t="s">
         <v>18</v>
       </c>
       <c r="J21" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="K21" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="L21">
-        <v>600</v>
+        <v>492</v>
       </c>
       <c r="M21">
-        <v>600</v>
+        <v>492</v>
       </c>
     </row>
     <row r="22" spans="1:13">
       <c r="A22" s="1">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B22" s="2">
-        <v>44652</v>
+        <v>44624</v>
       </c>
       <c r="C22" t="s">
         <v>12</v>
@@ -1502,77 +1565,77 @@
         <v>17</v>
       </c>
       <c r="F22" s="2">
-        <v>44694</v>
+        <v>44664</v>
       </c>
       <c r="G22">
-        <v>5.79</v>
+        <v>1.57</v>
       </c>
       <c r="H22">
-        <v>16.07</v>
+        <v>15.05</v>
       </c>
       <c r="I22" t="s">
         <v>18</v>
       </c>
       <c r="J22" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="K22" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="L22">
-        <v>1700</v>
+        <v>100</v>
       </c>
       <c r="M22">
-        <v>82</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:13">
       <c r="A23" s="1">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B23" s="2">
-        <v>44645</v>
+        <v>44629</v>
       </c>
       <c r="C23" t="s">
         <v>12</v>
       </c>
       <c r="D23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E23" t="s">
         <v>17</v>
       </c>
       <c r="F23" s="2">
-        <v>44687</v>
+        <v>44670</v>
       </c>
       <c r="G23">
-        <v>3.85</v>
+        <v>1.6</v>
       </c>
       <c r="H23">
-        <v>30.38</v>
+        <v>13.84</v>
       </c>
       <c r="I23" t="s">
         <v>18</v>
       </c>
       <c r="J23" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="K23" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="L23">
-        <v>1700</v>
+        <v>1150</v>
       </c>
       <c r="M23">
-        <v>1700</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="24" spans="1:13">
       <c r="A24" s="1">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B24" s="2">
-        <v>44645</v>
+        <v>44629</v>
       </c>
       <c r="C24" t="s">
         <v>12</v>
@@ -1584,118 +1647,118 @@
         <v>17</v>
       </c>
       <c r="F24" s="2">
-        <v>44687</v>
+        <v>44670</v>
       </c>
       <c r="G24">
-        <v>3.85</v>
+        <v>1.55</v>
       </c>
       <c r="H24">
-        <v>30.38</v>
+        <v>13.84</v>
       </c>
       <c r="I24" t="s">
         <v>18</v>
       </c>
       <c r="J24" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="K24" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="L24">
-        <v>448</v>
+        <v>1600</v>
       </c>
       <c r="M24">
-        <v>448</v>
+        <v>620</v>
       </c>
     </row>
     <row r="25" spans="1:13">
       <c r="A25" s="1">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B25" s="2">
-        <v>44616</v>
+        <v>44629</v>
       </c>
       <c r="C25" t="s">
         <v>12</v>
       </c>
       <c r="D25" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E25" t="s">
         <v>17</v>
       </c>
       <c r="F25" s="2">
-        <v>44658</v>
+        <v>44670</v>
       </c>
       <c r="G25">
-        <v>0.1</v>
+        <v>1.35</v>
       </c>
       <c r="H25">
-        <v>10.24</v>
+        <v>15.65</v>
       </c>
       <c r="I25" t="s">
         <v>18</v>
       </c>
       <c r="J25" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="K25" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="L25">
-        <v>864</v>
+        <v>1600</v>
       </c>
       <c r="M25">
-        <v>864</v>
+        <v>1600</v>
       </c>
     </row>
     <row r="26" spans="1:13">
       <c r="A26" s="1">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B26" s="2">
-        <v>44616</v>
+        <v>44631</v>
       </c>
       <c r="C26" t="s">
         <v>12</v>
       </c>
       <c r="D26" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E26" t="s">
         <v>17</v>
       </c>
       <c r="F26" s="2">
-        <v>44658</v>
+        <v>44673</v>
       </c>
       <c r="G26">
-        <v>0.1</v>
+        <v>1.29</v>
       </c>
       <c r="H26">
-        <v>10.24</v>
+        <v>14.36</v>
       </c>
       <c r="I26" t="s">
         <v>18</v>
       </c>
       <c r="J26" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="K26" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="L26">
-        <v>400</v>
+        <v>1600</v>
       </c>
       <c r="M26">
-        <v>400</v>
+        <v>1600</v>
       </c>
     </row>
     <row r="27" spans="1:13">
       <c r="A27" s="1">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B27" s="2">
-        <v>44629</v>
+        <v>44651</v>
       </c>
       <c r="C27" t="s">
         <v>12</v>
@@ -1707,77 +1770,77 @@
         <v>17</v>
       </c>
       <c r="F27" s="2">
-        <v>44670</v>
+        <v>44693</v>
       </c>
       <c r="G27">
-        <v>11.24</v>
+        <v>0.8699999999999999</v>
       </c>
       <c r="H27">
-        <v>13.03</v>
+        <v>15.41</v>
       </c>
       <c r="I27" t="s">
         <v>18</v>
       </c>
       <c r="J27" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="K27" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="L27">
-        <v>409</v>
+        <v>544</v>
       </c>
       <c r="M27">
-        <v>309</v>
+        <v>544</v>
       </c>
     </row>
     <row r="28" spans="1:13">
       <c r="A28" s="1">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B28" s="2">
-        <v>44616</v>
+        <v>44651</v>
       </c>
       <c r="C28" t="s">
         <v>12</v>
       </c>
       <c r="D28" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E28" t="s">
         <v>17</v>
       </c>
       <c r="F28" s="2">
-        <v>44658</v>
+        <v>44693</v>
       </c>
       <c r="G28">
-        <v>1</v>
+        <v>0.8699999999999999</v>
       </c>
       <c r="H28">
-        <v>18.98</v>
+        <v>15.41</v>
       </c>
       <c r="I28" t="s">
         <v>18</v>
       </c>
       <c r="J28" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="K28" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="L28">
-        <v>100</v>
+        <v>3300</v>
       </c>
       <c r="M28">
-        <v>100</v>
+        <v>2900</v>
       </c>
     </row>
     <row r="29" spans="1:13">
       <c r="A29" s="1">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B29" s="2">
-        <v>44615</v>
+        <v>44629</v>
       </c>
       <c r="C29" t="s">
         <v>12</v>
@@ -1789,145 +1852,145 @@
         <v>17</v>
       </c>
       <c r="F29" s="2">
-        <v>44657</v>
+        <v>44670</v>
       </c>
       <c r="G29">
-        <v>0.23</v>
+        <v>2.9</v>
       </c>
       <c r="H29">
-        <v>16.83</v>
+        <v>20.73</v>
       </c>
       <c r="I29" t="s">
         <v>18</v>
       </c>
       <c r="J29" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="K29" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="L29">
-        <v>700</v>
+        <v>1300</v>
       </c>
       <c r="M29">
-        <v>400</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="30" spans="1:13">
       <c r="A30" s="1">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B30" s="2">
-        <v>44651</v>
+        <v>44623</v>
       </c>
       <c r="C30" t="s">
         <v>12</v>
       </c>
       <c r="D30" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E30" t="s">
         <v>17</v>
       </c>
       <c r="F30" s="2">
-        <v>45016</v>
+        <v>44663</v>
       </c>
       <c r="G30">
-        <v>0.5</v>
+        <v>7.199999999999999</v>
       </c>
       <c r="H30">
-        <v>18.86</v>
+        <v>17.65</v>
       </c>
       <c r="I30" t="s">
         <v>18</v>
       </c>
       <c r="J30" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="K30" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="L30">
-        <v>1500</v>
+        <v>350</v>
       </c>
       <c r="M30">
-        <v>1500</v>
+        <v>350</v>
       </c>
     </row>
     <row r="31" spans="1:13">
       <c r="A31" s="1">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B31" s="2">
-        <v>44651</v>
+        <v>44631</v>
       </c>
       <c r="C31" t="s">
         <v>12</v>
       </c>
       <c r="D31" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E31" t="s">
         <v>17</v>
       </c>
       <c r="F31" s="2">
-        <v>45016</v>
+        <v>44673</v>
       </c>
       <c r="G31">
-        <v>0.5</v>
+        <v>6.84</v>
       </c>
       <c r="H31">
-        <v>18.86</v>
+        <v>16.99</v>
       </c>
       <c r="I31" t="s">
         <v>18</v>
       </c>
       <c r="J31" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="K31" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="L31">
-        <v>700</v>
+        <v>100</v>
       </c>
       <c r="M31">
-        <v>700</v>
+        <v>100</v>
       </c>
     </row>
     <row r="32" spans="1:13">
       <c r="A32" s="1">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B32" s="2">
-        <v>44651</v>
+        <v>44629</v>
       </c>
       <c r="C32" t="s">
         <v>12</v>
       </c>
       <c r="D32" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E32" t="s">
         <v>17</v>
       </c>
       <c r="F32" s="2">
-        <v>45016</v>
+        <v>44670</v>
       </c>
       <c r="G32">
-        <v>0.5</v>
+        <v>6.84</v>
       </c>
       <c r="H32">
-        <v>18.86</v>
+        <v>16.33</v>
       </c>
       <c r="I32" t="s">
         <v>18</v>
       </c>
       <c r="J32" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="K32" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="L32">
         <v>600</v>
@@ -1938,7 +2001,7 @@
     </row>
     <row r="33" spans="1:13">
       <c r="A33" s="1">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B33" s="2">
         <v>44652</v>
@@ -1947,83 +2010,83 @@
         <v>12</v>
       </c>
       <c r="D33" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E33" t="s">
         <v>17</v>
       </c>
       <c r="F33" s="2">
-        <v>45016</v>
+        <v>44694</v>
       </c>
       <c r="G33">
-        <v>0.5</v>
+        <v>5.79</v>
       </c>
       <c r="H33">
-        <v>18.83</v>
+        <v>16.07</v>
       </c>
       <c r="I33" t="s">
         <v>18</v>
       </c>
       <c r="J33" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="K33" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="L33">
-        <v>2500</v>
+        <v>1700</v>
       </c>
       <c r="M33">
-        <v>1400</v>
+        <v>82</v>
       </c>
     </row>
     <row r="34" spans="1:13">
       <c r="A34" s="1">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="B34" s="2">
-        <v>44652</v>
+        <v>44645</v>
       </c>
       <c r="C34" t="s">
         <v>12</v>
       </c>
       <c r="D34" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E34" t="s">
         <v>17</v>
       </c>
       <c r="F34" s="2">
-        <v>44741</v>
+        <v>44687</v>
       </c>
       <c r="G34">
-        <v>0.5</v>
+        <v>3.85</v>
       </c>
       <c r="H34">
-        <v>24.32</v>
+        <v>30.38</v>
       </c>
       <c r="I34" t="s">
         <v>18</v>
       </c>
       <c r="J34" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="K34" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="L34">
-        <v>4400</v>
+        <v>1700</v>
       </c>
       <c r="M34">
-        <v>4400</v>
+        <v>1700</v>
       </c>
     </row>
     <row r="35" spans="1:13">
       <c r="A35" s="1">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B35" s="2">
-        <v>44629</v>
+        <v>44645</v>
       </c>
       <c r="C35" t="s">
         <v>12</v>
@@ -2035,118 +2098,118 @@
         <v>17</v>
       </c>
       <c r="F35" s="2">
-        <v>44670</v>
+        <v>44687</v>
       </c>
       <c r="G35">
-        <v>0.03</v>
+        <v>3.85</v>
       </c>
       <c r="H35">
-        <v>28.55</v>
+        <v>30.38</v>
       </c>
       <c r="I35" t="s">
         <v>18</v>
       </c>
       <c r="J35" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="K35" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="L35">
-        <v>14585</v>
+        <v>448</v>
       </c>
       <c r="M35">
-        <v>7557</v>
+        <v>448</v>
       </c>
     </row>
     <row r="36" spans="1:13">
       <c r="A36" s="1">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="B36" s="2">
-        <v>44629</v>
+        <v>44616</v>
       </c>
       <c r="C36" t="s">
         <v>12</v>
       </c>
       <c r="D36" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E36" t="s">
         <v>17</v>
       </c>
       <c r="F36" s="2">
-        <v>44670</v>
+        <v>44658</v>
       </c>
       <c r="G36">
-        <v>0.12</v>
+        <v>0.1</v>
       </c>
       <c r="H36">
-        <v>39.25</v>
+        <v>10.24</v>
       </c>
       <c r="I36" t="s">
         <v>18</v>
       </c>
       <c r="J36" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="K36" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="L36">
-        <v>18900</v>
+        <v>864</v>
       </c>
       <c r="M36">
-        <v>18900</v>
+        <v>864</v>
       </c>
     </row>
     <row r="37" spans="1:13">
       <c r="A37" s="1">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="B37" s="2">
-        <v>44627</v>
+        <v>44616</v>
       </c>
       <c r="C37" t="s">
         <v>12</v>
       </c>
       <c r="D37" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E37" t="s">
         <v>17</v>
       </c>
       <c r="F37" s="2">
-        <v>44665</v>
+        <v>44658</v>
       </c>
       <c r="G37">
-        <v>0.12</v>
+        <v>0.1</v>
       </c>
       <c r="H37">
-        <v>38.67</v>
+        <v>10.24</v>
       </c>
       <c r="I37" t="s">
         <v>18</v>
       </c>
       <c r="J37" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="K37" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="L37">
-        <v>3800</v>
+        <v>400</v>
       </c>
       <c r="M37">
-        <v>3800</v>
+        <v>400</v>
       </c>
     </row>
     <row r="38" spans="1:13">
       <c r="A38" s="1">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="B38" s="2">
-        <v>44624</v>
+        <v>44629</v>
       </c>
       <c r="C38" t="s">
         <v>12</v>
@@ -2158,77 +2221,77 @@
         <v>17</v>
       </c>
       <c r="F38" s="2">
-        <v>44664</v>
+        <v>44670</v>
       </c>
       <c r="G38">
-        <v>0.12</v>
+        <v>11.24</v>
       </c>
       <c r="H38">
-        <v>38.44</v>
+        <v>13.03</v>
       </c>
       <c r="I38" t="s">
         <v>18</v>
       </c>
       <c r="J38" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="K38" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L38">
-        <v>1899</v>
+        <v>409</v>
       </c>
       <c r="M38">
-        <v>1899</v>
+        <v>309</v>
       </c>
     </row>
     <row r="39" spans="1:13">
       <c r="A39" s="1">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="B39" s="2">
-        <v>44624</v>
+        <v>44616</v>
       </c>
       <c r="C39" t="s">
         <v>12</v>
       </c>
       <c r="D39" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E39" t="s">
         <v>17</v>
       </c>
       <c r="F39" s="2">
-        <v>44664</v>
+        <v>44658</v>
       </c>
       <c r="G39">
-        <v>0.12</v>
+        <v>1</v>
       </c>
       <c r="H39">
-        <v>38.44</v>
+        <v>18.98</v>
       </c>
       <c r="I39" t="s">
         <v>18</v>
       </c>
       <c r="J39" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="K39" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="L39">
-        <v>3633</v>
+        <v>100</v>
       </c>
       <c r="M39">
-        <v>3633</v>
+        <v>100</v>
       </c>
     </row>
     <row r="40" spans="1:13">
       <c r="A40" s="1">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="B40" s="2">
-        <v>44652</v>
+        <v>44566</v>
       </c>
       <c r="C40" t="s">
         <v>12</v>
@@ -2240,33 +2303,33 @@
         <v>17</v>
       </c>
       <c r="F40" s="2">
-        <v>44693</v>
+        <v>44746</v>
       </c>
       <c r="G40">
         <v>0.5</v>
       </c>
       <c r="H40">
-        <v>55.66</v>
+        <v>12.07</v>
       </c>
       <c r="I40" t="s">
         <v>18</v>
       </c>
       <c r="J40" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="K40" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="L40">
-        <v>1400</v>
+        <v>1599</v>
       </c>
       <c r="M40">
-        <v>1400</v>
+        <v>1599</v>
       </c>
     </row>
     <row r="41" spans="1:13">
       <c r="A41" s="1">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="B41" s="2">
         <v>44652</v>
@@ -2281,77 +2344,77 @@
         <v>17</v>
       </c>
       <c r="F41" s="2">
-        <v>44693</v>
+        <v>44838</v>
       </c>
       <c r="G41">
         <v>0.5</v>
       </c>
       <c r="H41">
-        <v>55.66</v>
+        <v>10.18</v>
       </c>
       <c r="I41" t="s">
         <v>18</v>
       </c>
       <c r="J41" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="K41" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="L41">
-        <v>1300</v>
+        <v>1500</v>
       </c>
       <c r="M41">
-        <v>1300</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="42" spans="1:13">
       <c r="A42" s="1">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="B42" s="2">
-        <v>44652</v>
+        <v>44615</v>
       </c>
       <c r="C42" t="s">
         <v>12</v>
       </c>
       <c r="D42" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E42" t="s">
         <v>17</v>
       </c>
       <c r="F42" s="2">
-        <v>44693</v>
+        <v>44657</v>
       </c>
       <c r="G42">
-        <v>0.5</v>
+        <v>0.23</v>
       </c>
       <c r="H42">
-        <v>55.66</v>
+        <v>16.83</v>
       </c>
       <c r="I42" t="s">
         <v>18</v>
       </c>
       <c r="J42" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="K42" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="L42">
-        <v>1100</v>
+        <v>700</v>
       </c>
       <c r="M42">
-        <v>1100</v>
+        <v>400</v>
       </c>
     </row>
     <row r="43" spans="1:13">
       <c r="A43" s="1">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="B43" s="2">
-        <v>44652</v>
+        <v>44651</v>
       </c>
       <c r="C43" t="s">
         <v>12</v>
@@ -2363,36 +2426,36 @@
         <v>17</v>
       </c>
       <c r="F43" s="2">
-        <v>44693</v>
+        <v>45016</v>
       </c>
       <c r="G43">
         <v>0.5</v>
       </c>
       <c r="H43">
-        <v>55.66</v>
+        <v>18.86</v>
       </c>
       <c r="I43" t="s">
         <v>18</v>
       </c>
       <c r="J43" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K43" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="L43">
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="M43">
-        <v>1000</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="44" spans="1:13">
       <c r="A44" s="1">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="B44" s="2">
-        <v>44652</v>
+        <v>44651</v>
       </c>
       <c r="C44" t="s">
         <v>12</v>
@@ -2404,68 +2467,847 @@
         <v>17</v>
       </c>
       <c r="F44" s="2">
-        <v>44693</v>
+        <v>45016</v>
       </c>
       <c r="G44">
         <v>0.5</v>
       </c>
       <c r="H44">
-        <v>55.66</v>
+        <v>18.86</v>
       </c>
       <c r="I44" t="s">
         <v>18</v>
       </c>
       <c r="J44" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K44" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="L44">
-        <v>1000</v>
+        <v>700</v>
       </c>
       <c r="M44">
-        <v>900</v>
+        <v>700</v>
       </c>
     </row>
     <row r="45" spans="1:13">
       <c r="A45" s="1">
+        <v>52</v>
+      </c>
+      <c r="B45" s="2">
+        <v>44651</v>
+      </c>
+      <c r="C45" t="s">
+        <v>12</v>
+      </c>
+      <c r="D45" t="s">
+        <v>16</v>
+      </c>
+      <c r="E45" t="s">
+        <v>17</v>
+      </c>
+      <c r="F45" s="2">
+        <v>45016</v>
+      </c>
+      <c r="G45">
+        <v>0.5</v>
+      </c>
+      <c r="H45">
+        <v>18.86</v>
+      </c>
+      <c r="I45" t="s">
+        <v>18</v>
+      </c>
+      <c r="J45" t="s">
+        <v>35</v>
+      </c>
+      <c r="K45" t="s">
+        <v>83</v>
+      </c>
+      <c r="L45">
+        <v>600</v>
+      </c>
+      <c r="M45">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13">
+      <c r="A46" s="1">
+        <v>53</v>
+      </c>
+      <c r="B46" s="2">
+        <v>44652</v>
+      </c>
+      <c r="C46" t="s">
+        <v>12</v>
+      </c>
+      <c r="D46" t="s">
+        <v>16</v>
+      </c>
+      <c r="E46" t="s">
+        <v>17</v>
+      </c>
+      <c r="F46" s="2">
+        <v>45016</v>
+      </c>
+      <c r="G46">
+        <v>0.5</v>
+      </c>
+      <c r="H46">
+        <v>18.83</v>
+      </c>
+      <c r="I46" t="s">
+        <v>18</v>
+      </c>
+      <c r="J46" t="s">
+        <v>35</v>
+      </c>
+      <c r="K46" t="s">
+        <v>84</v>
+      </c>
+      <c r="L46">
+        <v>2500</v>
+      </c>
+      <c r="M46">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13">
+      <c r="A47" s="1">
+        <v>54</v>
+      </c>
+      <c r="B47" s="2">
+        <v>44652</v>
+      </c>
+      <c r="C47" t="s">
+        <v>12</v>
+      </c>
+      <c r="D47" t="s">
+        <v>16</v>
+      </c>
+      <c r="E47" t="s">
+        <v>17</v>
+      </c>
+      <c r="F47" s="2">
+        <v>45016</v>
+      </c>
+      <c r="G47">
+        <v>0.5</v>
+      </c>
+      <c r="H47">
+        <v>18.83</v>
+      </c>
+      <c r="I47" t="s">
+        <v>18</v>
+      </c>
+      <c r="J47" t="s">
+        <v>35</v>
+      </c>
+      <c r="K47" t="s">
+        <v>85</v>
+      </c>
+      <c r="L47">
+        <v>1500</v>
+      </c>
+      <c r="M47">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13">
+      <c r="A48" s="1">
+        <v>55</v>
+      </c>
+      <c r="B48" s="2">
+        <v>44652</v>
+      </c>
+      <c r="C48" t="s">
+        <v>12</v>
+      </c>
+      <c r="D48" t="s">
+        <v>16</v>
+      </c>
+      <c r="E48" t="s">
+        <v>17</v>
+      </c>
+      <c r="F48" s="2">
+        <v>45016</v>
+      </c>
+      <c r="G48">
+        <v>0.5</v>
+      </c>
+      <c r="H48">
+        <v>18.83</v>
+      </c>
+      <c r="I48" t="s">
+        <v>18</v>
+      </c>
+      <c r="J48" t="s">
+        <v>35</v>
+      </c>
+      <c r="K48" t="s">
+        <v>86</v>
+      </c>
+      <c r="L48">
+        <v>1000</v>
+      </c>
+      <c r="M48">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13">
+      <c r="A49" s="1">
+        <v>56</v>
+      </c>
+      <c r="B49" s="2">
+        <v>44652</v>
+      </c>
+      <c r="C49" t="s">
+        <v>12</v>
+      </c>
+      <c r="D49" t="s">
+        <v>16</v>
+      </c>
+      <c r="E49" t="s">
+        <v>17</v>
+      </c>
+      <c r="F49" s="2">
+        <v>45016</v>
+      </c>
+      <c r="G49">
+        <v>0.5</v>
+      </c>
+      <c r="H49">
+        <v>18.83</v>
+      </c>
+      <c r="I49" t="s">
+        <v>18</v>
+      </c>
+      <c r="J49" t="s">
+        <v>35</v>
+      </c>
+      <c r="K49" t="s">
+        <v>87</v>
+      </c>
+      <c r="L49">
+        <v>1000</v>
+      </c>
+      <c r="M49">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13">
+      <c r="A50" s="1">
+        <v>57</v>
+      </c>
+      <c r="B50" s="2">
+        <v>44652</v>
+      </c>
+      <c r="C50" t="s">
+        <v>12</v>
+      </c>
+      <c r="D50" t="s">
+        <v>16</v>
+      </c>
+      <c r="E50" t="s">
+        <v>17</v>
+      </c>
+      <c r="F50" s="2">
+        <v>45016</v>
+      </c>
+      <c r="G50">
+        <v>0.5</v>
+      </c>
+      <c r="H50">
+        <v>18.83</v>
+      </c>
+      <c r="I50" t="s">
+        <v>18</v>
+      </c>
+      <c r="J50" t="s">
+        <v>35</v>
+      </c>
+      <c r="K50" t="s">
+        <v>88</v>
+      </c>
+      <c r="L50">
+        <v>700</v>
+      </c>
+      <c r="M50">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13">
+      <c r="A51" s="1">
+        <v>58</v>
+      </c>
+      <c r="B51" s="2">
+        <v>44652</v>
+      </c>
+      <c r="C51" t="s">
+        <v>12</v>
+      </c>
+      <c r="D51" t="s">
+        <v>16</v>
+      </c>
+      <c r="E51" t="s">
+        <v>17</v>
+      </c>
+      <c r="F51" s="2">
+        <v>45016</v>
+      </c>
+      <c r="G51">
+        <v>0.5</v>
+      </c>
+      <c r="H51">
+        <v>18.83</v>
+      </c>
+      <c r="I51" t="s">
+        <v>18</v>
+      </c>
+      <c r="J51" t="s">
+        <v>35</v>
+      </c>
+      <c r="K51" t="s">
+        <v>89</v>
+      </c>
+      <c r="L51">
+        <v>500</v>
+      </c>
+      <c r="M51">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13">
+      <c r="A52" s="1">
+        <v>59</v>
+      </c>
+      <c r="B52" s="2">
+        <v>44652</v>
+      </c>
+      <c r="C52" t="s">
+        <v>12</v>
+      </c>
+      <c r="D52" t="s">
+        <v>16</v>
+      </c>
+      <c r="E52" t="s">
+        <v>17</v>
+      </c>
+      <c r="F52" s="2">
+        <v>45016</v>
+      </c>
+      <c r="G52">
+        <v>0.5</v>
+      </c>
+      <c r="H52">
+        <v>18.83</v>
+      </c>
+      <c r="I52" t="s">
+        <v>18</v>
+      </c>
+      <c r="J52" t="s">
+        <v>35</v>
+      </c>
+      <c r="K52" t="s">
+        <v>90</v>
+      </c>
+      <c r="L52">
+        <v>500</v>
+      </c>
+      <c r="M52">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13">
+      <c r="A53" s="1">
+        <v>60</v>
+      </c>
+      <c r="B53" s="2">
+        <v>44652</v>
+      </c>
+      <c r="C53" t="s">
+        <v>12</v>
+      </c>
+      <c r="D53" t="s">
+        <v>16</v>
+      </c>
+      <c r="E53" t="s">
+        <v>17</v>
+      </c>
+      <c r="F53" s="2">
+        <v>44741</v>
+      </c>
+      <c r="G53">
+        <v>0.5</v>
+      </c>
+      <c r="H53">
+        <v>24.32</v>
+      </c>
+      <c r="I53" t="s">
+        <v>18</v>
+      </c>
+      <c r="J53" t="s">
+        <v>36</v>
+      </c>
+      <c r="K53" t="s">
+        <v>91</v>
+      </c>
+      <c r="L53">
+        <v>4400</v>
+      </c>
+      <c r="M53">
+        <v>4400</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13">
+      <c r="A54" s="1">
+        <v>61</v>
+      </c>
+      <c r="B54" s="2">
+        <v>44629</v>
+      </c>
+      <c r="C54" t="s">
+        <v>12</v>
+      </c>
+      <c r="D54" t="s">
+        <v>14</v>
+      </c>
+      <c r="E54" t="s">
+        <v>17</v>
+      </c>
+      <c r="F54" s="2">
+        <v>44670</v>
+      </c>
+      <c r="G54">
+        <v>0.03</v>
+      </c>
+      <c r="H54">
+        <v>28.55</v>
+      </c>
+      <c r="I54" t="s">
+        <v>18</v>
+      </c>
+      <c r="J54" t="s">
+        <v>36</v>
+      </c>
+      <c r="K54" t="s">
+        <v>92</v>
+      </c>
+      <c r="L54">
+        <v>14585</v>
+      </c>
+      <c r="M54">
+        <v>7557</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13">
+      <c r="A55" s="1">
+        <v>68</v>
+      </c>
+      <c r="B55" s="2">
+        <v>44629</v>
+      </c>
+      <c r="C55" t="s">
+        <v>12</v>
+      </c>
+      <c r="D55" t="s">
+        <v>14</v>
+      </c>
+      <c r="E55" t="s">
+        <v>17</v>
+      </c>
+      <c r="F55" s="2">
+        <v>44670</v>
+      </c>
+      <c r="G55">
+        <v>0.12</v>
+      </c>
+      <c r="H55">
+        <v>39.25</v>
+      </c>
+      <c r="I55" t="s">
+        <v>18</v>
+      </c>
+      <c r="J55" t="s">
+        <v>37</v>
+      </c>
+      <c r="K55" t="s">
+        <v>93</v>
+      </c>
+      <c r="L55">
+        <v>18900</v>
+      </c>
+      <c r="M55">
+        <v>18900</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13">
+      <c r="A56" s="1">
+        <v>69</v>
+      </c>
+      <c r="B56" s="2">
+        <v>44627</v>
+      </c>
+      <c r="C56" t="s">
+        <v>12</v>
+      </c>
+      <c r="D56" t="s">
+        <v>14</v>
+      </c>
+      <c r="E56" t="s">
+        <v>17</v>
+      </c>
+      <c r="F56" s="2">
+        <v>44665</v>
+      </c>
+      <c r="G56">
+        <v>0.12</v>
+      </c>
+      <c r="H56">
+        <v>38.67</v>
+      </c>
+      <c r="I56" t="s">
+        <v>18</v>
+      </c>
+      <c r="J56" t="s">
+        <v>37</v>
+      </c>
+      <c r="K56" t="s">
+        <v>94</v>
+      </c>
+      <c r="L56">
+        <v>3800</v>
+      </c>
+      <c r="M56">
+        <v>3800</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13">
+      <c r="A57" s="1">
         <v>70</v>
       </c>
-      <c r="B45" s="2">
+      <c r="B57" s="2">
+        <v>44624</v>
+      </c>
+      <c r="C57" t="s">
+        <v>12</v>
+      </c>
+      <c r="D57" t="s">
+        <v>14</v>
+      </c>
+      <c r="E57" t="s">
+        <v>17</v>
+      </c>
+      <c r="F57" s="2">
+        <v>44664</v>
+      </c>
+      <c r="G57">
+        <v>0.12</v>
+      </c>
+      <c r="H57">
+        <v>38.44</v>
+      </c>
+      <c r="I57" t="s">
+        <v>18</v>
+      </c>
+      <c r="J57" t="s">
+        <v>37</v>
+      </c>
+      <c r="K57" t="s">
+        <v>95</v>
+      </c>
+      <c r="L57">
+        <v>1899</v>
+      </c>
+      <c r="M57">
+        <v>1899</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13">
+      <c r="A58" s="1">
+        <v>71</v>
+      </c>
+      <c r="B58" s="2">
+        <v>44624</v>
+      </c>
+      <c r="C58" t="s">
+        <v>12</v>
+      </c>
+      <c r="D58" t="s">
+        <v>14</v>
+      </c>
+      <c r="E58" t="s">
+        <v>17</v>
+      </c>
+      <c r="F58" s="2">
+        <v>44664</v>
+      </c>
+      <c r="G58">
+        <v>0.12</v>
+      </c>
+      <c r="H58">
+        <v>38.44</v>
+      </c>
+      <c r="I58" t="s">
+        <v>18</v>
+      </c>
+      <c r="J58" t="s">
+        <v>37</v>
+      </c>
+      <c r="K58" t="s">
+        <v>96</v>
+      </c>
+      <c r="L58">
+        <v>3633</v>
+      </c>
+      <c r="M58">
+        <v>3633</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13">
+      <c r="A59" s="1">
+        <v>72</v>
+      </c>
+      <c r="B59" s="2">
+        <v>44652</v>
+      </c>
+      <c r="C59" t="s">
+        <v>12</v>
+      </c>
+      <c r="D59" t="s">
+        <v>16</v>
+      </c>
+      <c r="E59" t="s">
+        <v>17</v>
+      </c>
+      <c r="F59" s="2">
+        <v>44693</v>
+      </c>
+      <c r="G59">
+        <v>0.5</v>
+      </c>
+      <c r="H59">
+        <v>55.66</v>
+      </c>
+      <c r="I59" t="s">
+        <v>18</v>
+      </c>
+      <c r="J59" t="s">
+        <v>38</v>
+      </c>
+      <c r="K59" t="s">
+        <v>97</v>
+      </c>
+      <c r="L59">
+        <v>1400</v>
+      </c>
+      <c r="M59">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13">
+      <c r="A60" s="1">
+        <v>73</v>
+      </c>
+      <c r="B60" s="2">
+        <v>44652</v>
+      </c>
+      <c r="C60" t="s">
+        <v>12</v>
+      </c>
+      <c r="D60" t="s">
+        <v>16</v>
+      </c>
+      <c r="E60" t="s">
+        <v>17</v>
+      </c>
+      <c r="F60" s="2">
+        <v>44693</v>
+      </c>
+      <c r="G60">
+        <v>0.5</v>
+      </c>
+      <c r="H60">
+        <v>55.66</v>
+      </c>
+      <c r="I60" t="s">
+        <v>18</v>
+      </c>
+      <c r="J60" t="s">
+        <v>38</v>
+      </c>
+      <c r="K60" t="s">
+        <v>98</v>
+      </c>
+      <c r="L60">
+        <v>1300</v>
+      </c>
+      <c r="M60">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13">
+      <c r="A61" s="1">
+        <v>74</v>
+      </c>
+      <c r="B61" s="2">
+        <v>44652</v>
+      </c>
+      <c r="C61" t="s">
+        <v>12</v>
+      </c>
+      <c r="D61" t="s">
+        <v>16</v>
+      </c>
+      <c r="E61" t="s">
+        <v>17</v>
+      </c>
+      <c r="F61" s="2">
+        <v>44693</v>
+      </c>
+      <c r="G61">
+        <v>0.5</v>
+      </c>
+      <c r="H61">
+        <v>55.66</v>
+      </c>
+      <c r="I61" t="s">
+        <v>18</v>
+      </c>
+      <c r="J61" t="s">
+        <v>38</v>
+      </c>
+      <c r="K61" t="s">
+        <v>99</v>
+      </c>
+      <c r="L61">
+        <v>1100</v>
+      </c>
+      <c r="M61">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13">
+      <c r="A62" s="1">
+        <v>75</v>
+      </c>
+      <c r="B62" s="2">
+        <v>44652</v>
+      </c>
+      <c r="C62" t="s">
+        <v>12</v>
+      </c>
+      <c r="D62" t="s">
+        <v>16</v>
+      </c>
+      <c r="E62" t="s">
+        <v>17</v>
+      </c>
+      <c r="F62" s="2">
+        <v>44693</v>
+      </c>
+      <c r="G62">
+        <v>0.5</v>
+      </c>
+      <c r="H62">
+        <v>55.66</v>
+      </c>
+      <c r="I62" t="s">
+        <v>18</v>
+      </c>
+      <c r="J62" t="s">
+        <v>38</v>
+      </c>
+      <c r="K62" t="s">
+        <v>100</v>
+      </c>
+      <c r="L62">
+        <v>1000</v>
+      </c>
+      <c r="M62">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13">
+      <c r="A63" s="1">
+        <v>76</v>
+      </c>
+      <c r="B63" s="2">
+        <v>44652</v>
+      </c>
+      <c r="C63" t="s">
+        <v>12</v>
+      </c>
+      <c r="D63" t="s">
+        <v>16</v>
+      </c>
+      <c r="E63" t="s">
+        <v>17</v>
+      </c>
+      <c r="F63" s="2">
+        <v>44693</v>
+      </c>
+      <c r="G63">
+        <v>0.5</v>
+      </c>
+      <c r="H63">
+        <v>55.66</v>
+      </c>
+      <c r="I63" t="s">
+        <v>18</v>
+      </c>
+      <c r="J63" t="s">
+        <v>38</v>
+      </c>
+      <c r="K63" t="s">
+        <v>101</v>
+      </c>
+      <c r="L63">
+        <v>1000</v>
+      </c>
+      <c r="M63">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13">
+      <c r="A64" s="1">
+        <v>83</v>
+      </c>
+      <c r="B64" s="2">
         <v>44645</v>
       </c>
-      <c r="C45" t="s">
-        <v>12</v>
-      </c>
-      <c r="D45" t="s">
-        <v>14</v>
-      </c>
-      <c r="E45" t="s">
-        <v>17</v>
-      </c>
-      <c r="F45" s="2">
+      <c r="C64" t="s">
+        <v>12</v>
+      </c>
+      <c r="D64" t="s">
+        <v>14</v>
+      </c>
+      <c r="E64" t="s">
+        <v>17</v>
+      </c>
+      <c r="F64" s="2">
         <v>44687</v>
       </c>
-      <c r="G45">
+      <c r="G64">
         <v>0.08</v>
       </c>
-      <c r="H45">
+      <c r="H64">
         <v>96.67</v>
       </c>
-      <c r="I45" t="s">
-        <v>18</v>
-      </c>
-      <c r="J45" t="s">
-        <v>37</v>
-      </c>
-      <c r="K45" t="s">
-        <v>81</v>
-      </c>
-      <c r="L45">
+      <c r="I64" t="s">
+        <v>18</v>
+      </c>
+      <c r="J64" t="s">
+        <v>39</v>
+      </c>
+      <c r="K64" t="s">
+        <v>102</v>
+      </c>
+      <c r="L64">
         <v>46362</v>
       </c>
-      <c r="M45">
+      <c r="M64">
         <v>33856</v>
       </c>
     </row>

</xml_diff>